<commit_message>
fix tests and nist groups error
</commit_message>
<xml_diff>
--- a/tests/expected_results/expected_excel_results.xlsx
+++ b/tests/expected_results/expected_excel_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emeth/mappings-explorer/tests/expected_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683416DA-C89D-6345-A9D4-B70C631DAC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF44C17-72BE-2243-99A4-538E54B31488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{03E5BEE8-75C6-0942-B5C2-F473EDA01C70}"/>
+    <workbookView xWindow="800" yWindow="13200" windowWidth="29880" windowHeight="7440" xr2:uid="{03E5BEE8-75C6-0942-B5C2-F473EDA01C70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>mapping_framework_version</t>
   </si>
   <si>
-    <t>mapping_framework_version_schema</t>
-  </si>
-  <si>
     <t>T1137</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>nist_800_53</t>
   </si>
   <si>
-    <t>FRAMEWORK_VERSION</t>
-  </si>
-  <si>
     <t>T1137.002</t>
   </si>
   <si>
@@ -126,6 +120,12 @@
   </si>
   <si>
     <t>10/27/2021</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>complete</t>
   </si>
 </sst>
 </file>
@@ -134,7 +134,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="166" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -181,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DF0C68-A4A2-2047-B70A-7BE33C1569D3}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="J5:K6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,15 +508,16 @@
     <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -545,143 +546,143 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
       </c>
       <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>28</v>
+      <c r="I2" t="s">
+        <v>29</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
         <v>22</v>
       </c>
-      <c r="N2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2">
+      <c r="P2">
         <v>1</v>
-      </c>
-      <c r="P2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
       </c>
       <c r="H3" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>28</v>
+      <c r="I3" t="s">
+        <v>29</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
         <v>22</v>
       </c>
-      <c r="N3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3">
+      <c r="P3">
         <v>1</v>
       </c>
-      <c r="P3" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J4" s="1"/>
       <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J5" s="3"/>
       <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J6" s="3"/>
       <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J8" s="2"/>
       <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Update unified schema (#29)
* add status and non-mappable mappings

* mapping_types and group changes

* fix file structures

* update unified schema, export new parsed mappings

* do not allow 'group' to be null

* fix tests and nist groups error

* site-builder fixes

---------

Co-authored-by: Eva <emeth.ctr@kr.af.mil>
</commit_message>
<xml_diff>
--- a/tests/expected_results/expected_excel_results.xlsx
+++ b/tests/expected_results/expected_excel_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emeth/mappings-explorer/tests/expected_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683416DA-C89D-6345-A9D4-B70C631DAC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF44C17-72BE-2243-99A4-538E54B31488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{03E5BEE8-75C6-0942-B5C2-F473EDA01C70}"/>
+    <workbookView xWindow="800" yWindow="13200" windowWidth="29880" windowHeight="7440" xr2:uid="{03E5BEE8-75C6-0942-B5C2-F473EDA01C70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>mapping_framework_version</t>
   </si>
   <si>
-    <t>mapping_framework_version_schema</t>
-  </si>
-  <si>
     <t>T1137</t>
   </si>
   <si>
@@ -110,9 +107,6 @@
     <t>nist_800_53</t>
   </si>
   <si>
-    <t>FRAMEWORK_VERSION</t>
-  </si>
-  <si>
     <t>T1137.002</t>
   </si>
   <si>
@@ -126,6 +120,12 @@
   </si>
   <si>
     <t>10/27/2021</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>complete</t>
   </si>
 </sst>
 </file>
@@ -134,7 +134,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="166" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -181,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -499,8 +499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84DF0C68-A4A2-2047-B70A-7BE33C1569D3}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="J5:K6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,15 +508,16 @@
     <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" customWidth="1"/>
+    <col min="9" max="9" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -545,143 +546,143 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
       </c>
       <c r="H2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>28</v>
+      <c r="I2" t="s">
+        <v>29</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
         <v>22</v>
       </c>
-      <c r="N2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2">
+      <c r="P2">
         <v>1</v>
-      </c>
-      <c r="P2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
       </c>
       <c r="H3" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>28</v>
+      <c r="I3" t="s">
+        <v>29</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" t="s">
         <v>22</v>
       </c>
-      <c r="N3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O3">
+      <c r="P3">
         <v>1</v>
       </c>
-      <c r="P3" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J4" s="1"/>
       <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J5" s="3"/>
       <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J6" s="3"/>
       <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J8" s="2"/>
       <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J9" s="2"/>
       <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
MAPEX-123: Update terminology in CLI Tools (#49)
* change 'group' to 'capability_group' when parsing mappings

* change json schema and update exports

* fix tests

* fix tests

* update terminology in site_builder

* fix template name

---------

Co-authored-by: Eva <emeth.ctr@kr.af.mil>
</commit_message>
<xml_diff>
--- a/tests/expected_results/expected_excel_results.xlsx
+++ b/tests/expected_results/expected_excel_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emeth/mappings-explorer/tests/expected_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF44C17-72BE-2243-99A4-538E54B31488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5BFAA2-8563-4F4F-A3BD-36AE241791BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="800" yWindow="13200" windowWidth="29880" windowHeight="7440" xr2:uid="{03E5BEE8-75C6-0942-B5C2-F473EDA01C70}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>comments</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>complete</t>
+  </si>
+  <si>
+    <t>capability_group</t>
   </si>
 </sst>
 </file>
@@ -500,7 +503,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,7 +546,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="I1" t="s">
         <v>28</v>

</xml_diff>